<commit_message>
ver 0.118 - PDF form ažuriran
</commit_message>
<xml_diff>
--- a/backup_data.xlsx
+++ b/backup_data.xlsx
@@ -8,23 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mihas\Programming\Python\Projects\PutniNalozi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C69ABC7-8D1E-4373-B093-14BB454002B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26CD96C3-B2C5-4FB3-A321-AC81724A319A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users_export" sheetId="1" r:id="rId1"/>
     <sheet name="Company_export" sheetId="2" r:id="rId2"/>
     <sheet name="Warrants_export" sheetId="3" r:id="rId3"/>
     <sheet name="Users_input" sheetId="4" r:id="rId4"/>
-    <sheet name="Warrants_input" sheetId="5" r:id="rId5"/>
+    <sheet name="Company_input" sheetId="6" r:id="rId5"/>
+    <sheet name="Warrants_input" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="157">
   <si>
     <t>id</t>
   </si>
@@ -465,6 +466,36 @@
   </si>
   <si>
     <t>Ivan Ivo</t>
+  </si>
+  <si>
+    <t>default_vehicle</t>
+  </si>
+  <si>
+    <t>cashier_email</t>
+  </si>
+  <si>
+    <t>CEO</t>
+  </si>
+  <si>
+    <t>stamparijabeograd.com</t>
+  </si>
+  <si>
+    <t>blagajnik@gmail.com</t>
+  </si>
+  <si>
+    <t>Elon Musk</t>
+  </si>
+  <si>
+    <t>blagajnik1@gmail.com</t>
+  </si>
+  <si>
+    <t>blagajnik2@gmail.com</t>
+  </si>
+  <si>
+    <t>Vladimir Simić</t>
+  </si>
+  <si>
+    <t>Vukadinac</t>
   </si>
 </sst>
 </file>
@@ -474,7 +505,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -507,6 +538,14 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -516,7 +555,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -584,11 +623,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -606,8 +657,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -910,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1857,10 +1913,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1873,7 +1929,7 @@
     <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1901,8 +1957,11 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1930,8 +1989,11 @@
       <c r="I2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1959,8 +2021,11 @@
       <c r="I3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1988,8 +2053,11 @@
       <c r="I4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2017,8 +2085,11 @@
       <c r="I5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2046,8 +2117,11 @@
       <c r="I6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2075,8 +2149,11 @@
       <c r="I7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2104,8 +2181,11 @@
       <c r="I8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2133,8 +2213,11 @@
       <c r="I9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2162,8 +2245,11 @@
       <c r="I10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2191,8 +2277,11 @@
       <c r="I11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2220,8 +2309,11 @@
       <c r="I12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2248,6 +2340,9 @@
       </c>
       <c r="I13">
         <v>1</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2256,11 +2351,219 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01786EBB-8240-42B9-A260-165FA80D2A1E}">
+  <dimension ref="A1:O4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2">
+        <v>24</v>
+      </c>
+      <c r="E2">
+        <v>32300</v>
+      </c>
+      <c r="F2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2">
+        <v>123456789</v>
+      </c>
+      <c r="I2">
+        <v>12345677</v>
+      </c>
+      <c r="J2" t="s">
+        <v>97</v>
+      </c>
+      <c r="K2" t="s">
+        <v>98</v>
+      </c>
+      <c r="L2">
+        <v>38132771000</v>
+      </c>
+      <c r="M2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="O2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3">
+        <v>212</v>
+      </c>
+      <c r="E3">
+        <v>32300</v>
+      </c>
+      <c r="F3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H3">
+        <v>123456789</v>
+      </c>
+      <c r="I3">
+        <v>12345678</v>
+      </c>
+      <c r="J3" t="s">
+        <v>102</v>
+      </c>
+      <c r="K3" t="s">
+        <v>103</v>
+      </c>
+      <c r="L3">
+        <v>38132770311</v>
+      </c>
+      <c r="M3" t="s">
+        <v>104</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="O3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4">
+        <v>36</v>
+      </c>
+      <c r="E4">
+        <v>11000</v>
+      </c>
+      <c r="F4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G4" t="s">
+        <v>108</v>
+      </c>
+      <c r="H4">
+        <v>108783967</v>
+      </c>
+      <c r="I4">
+        <v>63700061</v>
+      </c>
+      <c r="J4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K4" t="s">
+        <v>110</v>
+      </c>
+      <c r="L4" t="s">
+        <v>111</v>
+      </c>
+      <c r="M4" t="s">
+        <v>112</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="O4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="N2" r:id="rId1" xr:uid="{DC24830A-C179-4B05-9734-8EA9C721725A}"/>
+    <hyperlink ref="N3" r:id="rId2" xr:uid="{45F69F34-FCDE-4662-87A5-1EFB72CFEEC6}"/>
+    <hyperlink ref="N4" r:id="rId3" xr:uid="{0B76A137-F307-47CD-9283-6F84430FCBEE}"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ver 0.213 dodata opcija 'dodaj trošak'
</commit_message>
<xml_diff>
--- a/backup_data.xlsx
+++ b/backup_data.xlsx
@@ -8,24 +8,38 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mihas\Programming\Python\Projects\PutniNalozi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05791CA6-B1E0-46A0-93AA-6C968E248E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B3F7D3-B2CC-4773-AA3A-53604346ED2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users_export" sheetId="1" r:id="rId1"/>
     <sheet name="Company_export" sheetId="2" r:id="rId2"/>
     <sheet name="Warrants_export" sheetId="3" r:id="rId3"/>
     <sheet name="Users_input" sheetId="4" r:id="rId4"/>
-    <sheet name="Company_input" sheetId="6" r:id="rId5"/>
-    <sheet name="Warrants_input" sheetId="5" r:id="rId6"/>
+    <sheet name="Users_input (backup)" sheetId="7" r:id="rId5"/>
+    <sheet name="Company_input" sheetId="6" r:id="rId6"/>
+    <sheet name="Warrants_input" sheetId="5" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="183">
   <si>
     <t>id</t>
   </si>
@@ -502,6 +516,78 @@
   </si>
   <si>
     <t>Pomoćni radnik</t>
+  </si>
+  <si>
+    <t>CONNECT GRADNJA 011 DOO</t>
+  </si>
+  <si>
+    <t>ĆIRILA I METODIJA 2</t>
+  </si>
+  <si>
+    <t>blagajnik3@gmail.com</t>
+  </si>
+  <si>
+    <t>steslo@gmail.com</t>
+  </si>
+  <si>
+    <t>Slobodan</t>
+  </si>
+  <si>
+    <t>Stevanović</t>
+  </si>
+  <si>
+    <t>Pomoćnik tesara</t>
+  </si>
+  <si>
+    <t>đordej@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dejan </t>
+  </si>
+  <si>
+    <t>Đorđević</t>
+  </si>
+  <si>
+    <t>ljubomir.connect@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ljubomir </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mitrović </t>
+  </si>
+  <si>
+    <t>rajpen@gmail.com</t>
+  </si>
+  <si>
+    <t>pomoćni radnik</t>
+  </si>
+  <si>
+    <t>sampra@gmail.com</t>
+  </si>
+  <si>
+    <t>grefer@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pendyala </t>
+  </si>
+  <si>
+    <t>Rajashekhar</t>
+  </si>
+  <si>
+    <t>Prathipati</t>
+  </si>
+  <si>
+    <t>Sampath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fernandes </t>
+  </si>
+  <si>
+    <t>Greig Vincent</t>
+  </si>
+  <si>
+    <t>ef88c20087854a96.png</t>
   </si>
 </sst>
 </file>
@@ -1919,10 +2005,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1969,31 +2055,31 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>162</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>163</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>164</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>165</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -2001,31 +2087,31 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>166</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>167</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>168</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>165</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -2033,31 +2119,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>169</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>170</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>171</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>158</v>
       </c>
       <c r="H4" t="s">
         <v>26</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -2065,31 +2151,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>173</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5">
         <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -2097,31 +2183,31 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>174</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>178</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>179</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>37</v>
+        <v>158</v>
       </c>
       <c r="H6" t="s">
         <v>26</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -2129,513 +2215,997 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>175</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
-        <v>146</v>
+        <v>180</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>181</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>43</v>
+        <v>158</v>
       </c>
       <c r="H7" t="s">
         <v>26</v>
       </c>
       <c r="I7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I8">
-        <v>2</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
-        <v>53</v>
-      </c>
-      <c r="H9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9">
-        <v>2</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10">
-        <v>2</v>
-      </c>
-      <c r="G10" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" t="s">
-        <v>26</v>
-      </c>
-      <c r="I10">
-        <v>2</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11">
-        <v>2</v>
-      </c>
-      <c r="G11" t="s">
-        <v>62</v>
-      </c>
-      <c r="H11" t="s">
-        <v>26</v>
-      </c>
-      <c r="I11">
-        <v>2</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" t="s">
-        <v>65</v>
-      </c>
-      <c r="E12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12" t="s">
-        <v>66</v>
-      </c>
-      <c r="H12" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" t="s">
-        <v>70</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13" t="s">
-        <v>71</v>
-      </c>
-      <c r="H13" t="s">
-        <v>26</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" t="s">
-        <v>74</v>
-      </c>
-      <c r="E14" t="s">
-        <v>75</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14" t="s">
-        <v>157</v>
-      </c>
-      <c r="H14" t="s">
-        <v>20</v>
-      </c>
-      <c r="I14">
-        <v>3</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="C15" t="s">
-        <v>68</v>
-      </c>
-      <c r="D15" t="s">
-        <v>79</v>
-      </c>
-      <c r="E15" t="s">
-        <v>75</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15" t="s">
-        <v>158</v>
-      </c>
-      <c r="H15" t="s">
-        <v>26</v>
-      </c>
-      <c r="I15">
-        <v>3</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B14" r:id="rId1" xr:uid="{D0CE7649-F61E-4135-8362-A61B1467A603}"/>
-    <hyperlink ref="B15" r:id="rId2" xr:uid="{6DA991D7-BE62-43C9-9B3A-4685B9700178}"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01786EBB-8240-42B9-A260-165FA80D2A1E}">
-  <dimension ref="A1:O4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60D3F347-A6BA-4FAE-91A5-8F695274308A}">
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D2">
-        <v>24</v>
-      </c>
-      <c r="E2">
-        <v>32300</v>
-      </c>
-      <c r="F2" t="s">
-        <v>95</v>
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H2">
-        <v>123456789</v>
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
       </c>
       <c r="I2">
-        <v>12345677</v>
-      </c>
-      <c r="J2" t="s">
-        <v>97</v>
-      </c>
-      <c r="K2" t="s">
-        <v>98</v>
-      </c>
-      <c r="L2">
-        <v>38132771000</v>
-      </c>
-      <c r="M2" t="s">
-        <v>99</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="O2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D3">
-        <v>212</v>
-      </c>
-      <c r="E3">
-        <v>32300</v>
-      </c>
-      <c r="F3" t="s">
-        <v>95</v>
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>96</v>
-      </c>
-      <c r="H3">
-        <v>123456789</v>
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
       </c>
       <c r="I3">
-        <v>12345678</v>
-      </c>
-      <c r="J3" t="s">
-        <v>102</v>
-      </c>
-      <c r="K3" t="s">
-        <v>103</v>
-      </c>
-      <c r="L3">
-        <v>38132770311</v>
-      </c>
-      <c r="M3" t="s">
-        <v>104</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="O3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D4">
-        <v>36</v>
-      </c>
-      <c r="E4">
-        <v>11000</v>
-      </c>
-      <c r="F4" t="s">
-        <v>107</v>
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>108</v>
-      </c>
-      <c r="H4">
-        <v>108783967</v>
+        <v>25</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
       </c>
       <c r="I4">
-        <v>63700061</v>
-      </c>
-      <c r="J4" t="s">
-        <v>150</v>
-      </c>
-      <c r="K4" t="s">
-        <v>110</v>
-      </c>
-      <c r="L4" t="s">
-        <v>111</v>
-      </c>
-      <c r="M4" t="s">
-        <v>112</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="O4" t="s">
-        <v>152</v>
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s">
+        <v>146</v>
+      </c>
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>71</v>
+      </c>
+      <c r="H13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>157</v>
+      </c>
+      <c r="H14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>158</v>
+      </c>
+      <c r="H15" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15">
+        <v>3</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>162</v>
+      </c>
+      <c r="C16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" t="s">
+        <v>163</v>
+      </c>
+      <c r="E16" t="s">
+        <v>164</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>165</v>
+      </c>
+      <c r="H16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I16">
+        <v>4</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>166</v>
+      </c>
+      <c r="C17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E17" t="s">
+        <v>168</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>165</v>
+      </c>
+      <c r="H17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I17">
+        <v>4</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>169</v>
+      </c>
+      <c r="C18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" t="s">
+        <v>170</v>
+      </c>
+      <c r="E18" t="s">
+        <v>171</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>158</v>
+      </c>
+      <c r="H18" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18">
+        <v>4</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>172</v>
+      </c>
+      <c r="C19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" t="s">
+        <v>176</v>
+      </c>
+      <c r="E19" t="s">
+        <v>177</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>173</v>
+      </c>
+      <c r="H19" t="s">
+        <v>26</v>
+      </c>
+      <c r="I19">
+        <v>4</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>174</v>
+      </c>
+      <c r="C20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" t="s">
+        <v>178</v>
+      </c>
+      <c r="E20" t="s">
+        <v>179</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>158</v>
+      </c>
+      <c r="H20" t="s">
+        <v>26</v>
+      </c>
+      <c r="I20">
+        <v>4</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>175</v>
+      </c>
+      <c r="C21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" t="s">
+        <v>180</v>
+      </c>
+      <c r="E21" t="s">
+        <v>181</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>158</v>
+      </c>
+      <c r="H21" t="s">
+        <v>26</v>
+      </c>
+      <c r="I21">
+        <v>4</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N2" r:id="rId1" xr:uid="{DC24830A-C179-4B05-9734-8EA9C721725A}"/>
-    <hyperlink ref="N3" r:id="rId2" xr:uid="{45F69F34-FCDE-4662-87A5-1EFB72CFEEC6}"/>
-    <hyperlink ref="N4" r:id="rId3" xr:uid="{0B76A137-F307-47CD-9283-6F84430FCBEE}"/>
+    <hyperlink ref="B14" r:id="rId1" xr:uid="{AF4EE84D-1D1E-475F-9D19-94A1182FCDF8}"/>
+    <hyperlink ref="B15" r:id="rId2" xr:uid="{6FDA0D69-5F28-491F-9AB5-52CC3B90DC7A}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01786EBB-8240-42B9-A260-165FA80D2A1E}">
+  <dimension ref="A1:O5"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2">
+        <v>24</v>
+      </c>
+      <c r="E2">
+        <v>32300</v>
+      </c>
+      <c r="F2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2">
+        <v>123456789</v>
+      </c>
+      <c r="I2">
+        <v>12345677</v>
+      </c>
+      <c r="J2" t="s">
+        <v>97</v>
+      </c>
+      <c r="K2" t="s">
+        <v>98</v>
+      </c>
+      <c r="L2">
+        <v>38132771000</v>
+      </c>
+      <c r="M2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="O2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3">
+        <v>212</v>
+      </c>
+      <c r="E3">
+        <v>32300</v>
+      </c>
+      <c r="F3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H3">
+        <v>123456789</v>
+      </c>
+      <c r="I3">
+        <v>12345678</v>
+      </c>
+      <c r="J3" t="s">
+        <v>102</v>
+      </c>
+      <c r="K3" t="s">
+        <v>103</v>
+      </c>
+      <c r="L3">
+        <v>38132770311</v>
+      </c>
+      <c r="M3" t="s">
+        <v>104</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="O3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4">
+        <v>36</v>
+      </c>
+      <c r="E4">
+        <v>11000</v>
+      </c>
+      <c r="F4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G4" t="s">
+        <v>108</v>
+      </c>
+      <c r="H4">
+        <v>108783967</v>
+      </c>
+      <c r="I4">
+        <v>63700061</v>
+      </c>
+      <c r="J4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K4" t="s">
+        <v>110</v>
+      </c>
+      <c r="L4" t="s">
+        <v>111</v>
+      </c>
+      <c r="M4" t="s">
+        <v>112</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="O4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C5" t="s">
+        <v>160</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>11000</v>
+      </c>
+      <c r="F5" t="s">
+        <v>107</v>
+      </c>
+      <c r="G5" t="s">
+        <v>108</v>
+      </c>
+      <c r="H5">
+        <v>112762175</v>
+      </c>
+      <c r="I5">
+        <v>21734349</v>
+      </c>
+      <c r="K5" t="s">
+        <v>77</v>
+      </c>
+      <c r="L5">
+        <v>649194504</v>
+      </c>
+      <c r="M5" t="s">
+        <v>182</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="N2" r:id="rId1" xr:uid="{DC24830A-C179-4B05-9734-8EA9C721725A}"/>
+    <hyperlink ref="N3" r:id="rId2" xr:uid="{45F69F34-FCDE-4662-87A5-1EFB72CFEEC6}"/>
+    <hyperlink ref="N4" r:id="rId3" xr:uid="{0B76A137-F307-47CD-9283-6F84430FCBEE}"/>
+    <hyperlink ref="N5" r:id="rId4" xr:uid="{34D281A4-40BC-4B9D-AAAB-6AEF9F31C686}"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>

</xml_diff>

<commit_message>
ver 0.219 prilagođen kod za SQL
</commit_message>
<xml_diff>
--- a/backup_data.xlsx
+++ b/backup_data.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mihas\Programming\Python\Projects\PutniNalozi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B3F7D3-B2CC-4773-AA3A-53604346ED2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48450A56-9128-4A96-A191-5E76A3EB911E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users_export" sheetId="1" r:id="rId1"/>
     <sheet name="Company_export" sheetId="2" r:id="rId2"/>
     <sheet name="Warrants_export" sheetId="3" r:id="rId3"/>
-    <sheet name="Users_input" sheetId="4" r:id="rId4"/>
-    <sheet name="Users_input (backup)" sheetId="7" r:id="rId5"/>
+    <sheet name="Users_input (back up)" sheetId="4" r:id="rId4"/>
+    <sheet name="Users_input" sheetId="7" r:id="rId5"/>
     <sheet name="Company_input" sheetId="6" r:id="rId6"/>
     <sheet name="Warrants_input" sheetId="5" r:id="rId7"/>
   </sheets>
@@ -609,26 +609,36 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
     <font>
       <u/>
@@ -2007,7 +2017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -2254,8 +2264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60D3F347-A6BA-4FAE-91A5-8F695274308A}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>